<commit_message>
unit test for EORM
</commit_message>
<xml_diff>
--- a/testdata/title.xlsx
+++ b/testdata/title.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stephen/dev/workspaces/git/stephenfire/src/github.com/stephenfire/go-eorm/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20A79562-FA80-CF40-8AB3-3C5CB31C3195}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50597016-D302-A441-ACD8-61412EBB962A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6500" yWindow="4320" windowWidth="28100" windowHeight="17360" xr2:uid="{D6FFA577-0B41-9E4F-9795-21CC5A26DA9D}"/>
+    <workbookView xWindow="73120" yWindow="6540" windowWidth="28100" windowHeight="17360" xr2:uid="{D6FFA577-0B41-9E4F-9795-21CC5A26DA9D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -58,14 +58,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>没有第三级</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>空格</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>反斜杠\</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -78,7 +70,19 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>最后一列</t>
+    <t>第二级</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>name10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>name20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>空 格</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -125,12 +129,15 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -466,10 +473,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10C46AAB-3120-2742-9EF8-0439FD14DA81}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -501,37 +508,93 @@
         <v>4</v>
       </c>
       <c r="F2" s="1"/>
-      <c r="G2" s="1" t="s">
-        <v>5</v>
+      <c r="G2" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
         <v>6</v>
       </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
       <c r="E3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" t="s">
         <v>7</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="1"/>
+      <c r="C4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>13</v>
+      </c>
+      <c r="E4">
+        <v>14</v>
+      </c>
+      <c r="F4">
+        <v>15</v>
+      </c>
+      <c r="G4">
+        <v>16</v>
+      </c>
+      <c r="H4">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>23</v>
+      </c>
+      <c r="E5">
+        <v>24</v>
+      </c>
+      <c r="F5">
+        <v>25</v>
+      </c>
+      <c r="G5">
+        <v>26</v>
+      </c>
+      <c r="H5">
+        <v>27</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="5">
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="B1:B3"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:G3"/>
     <mergeCell ref="C1:H1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>